<commit_message>
Amador data through 2020-12-07
</commit_message>
<xml_diff>
--- a/Forecasts/Amador.xlsx
+++ b/Forecasts/Amador.xlsx
@@ -698,7 +698,7 @@
     <t xml:space="preserve">$time.of.run</t>
   </si>
   <si>
-    <t xml:space="preserve">[1] "2020-12-08 19:54:20"</t>
+    <t xml:space="preserve">[1] "2020-12-08 20:26:54"</t>
   </si>
   <si>
     <t xml:space="preserve">$LEMMA.version</t>
@@ -707,7 +707,7 @@
     <t xml:space="preserve">     version </t>
   </si>
   <si>
-    <t xml:space="preserve">"0.5.0.9015" </t>
+    <t xml:space="preserve">"0.5.0.9016" </t>
   </si>
 </sst>
 </file>

</xml_diff>